<commit_message>
Added special related achievements
</commit_message>
<xml_diff>
--- a/My Sets/Armour Force (Mega Duck)/Armour Force - Plan.xlsx
+++ b/My Sets/Armour Force (Mega Duck)/Armour Force - Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="635" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="635" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Game Dec" sheetId="16" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Achievements!$B$1:$G$172</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Achievements!$B$1:$G$174</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Checklist!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="72">
   <si>
     <t>Description</t>
   </si>
@@ -246,6 +246,18 @@
   </si>
   <si>
     <t>Highest score</t>
+  </si>
+  <si>
+    <t>Nothing Special Here</t>
+  </si>
+  <si>
+    <t>Defeat a boss without activating the special</t>
+  </si>
+  <si>
+    <t>Defeat a boss while the special is activated</t>
+  </si>
+  <si>
+    <t>Specialized Boss Slayer</t>
   </si>
 </sst>
 </file>
@@ -608,10 +620,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G175"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F2:F15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E17" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,21 +824,21 @@
         <v>54</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E9" s="7">
         <f>VLOOKUP(D9,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -834,20 +846,21 @@
         <v>54</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E10" s="7">
         <f>VLOOKUP(D10,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -855,61 +868,61 @@
         <v>54</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="7">
         <f>VLOOKUP(D11,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E12" s="7">
         <f>VLOOKUP(D12,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>65</v>
+        <v>54</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E13" s="7">
         <f>VLOOKUP(D13,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="5"/>
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
@@ -918,22 +931,21 @@
       <c r="B14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>66</v>
+      <c r="C14" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E14" s="7">
         <f>VLOOKUP(D14,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -941,115 +953,147 @@
         <v>35</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E15" s="7">
         <f>VLOOKUP(D15,Stats!$A$1:$B$10,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="7">
+        <f>VLOOKUP(D16,Stats!$A$1:$B$10,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="7">
+        <f>VLOOKUP(D17,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>25</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
-      <c r="D16" s="5"/>
-      <c r="G16"/>
-    </row>
-    <row r="17" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="D17" s="5"/>
-      <c r="G17"/>
-    </row>
-    <row r="18" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
-      <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
-      <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1183,13 +1227,13 @@
     </row>
     <row r="54" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="8"/>
-      <c r="C54" s="10"/>
+      <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="G54" s="5"/>
     </row>
     <row r="55" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="8"/>
-      <c r="C55" s="10"/>
+      <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="G55" s="5"/>
     </row>
@@ -1219,13 +1263,13 @@
     </row>
     <row r="60" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
-      <c r="C60" s="5"/>
+      <c r="C60" s="10"/>
       <c r="D60" s="5"/>
       <c r="G60" s="5"/>
     </row>
     <row r="61" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="8"/>
-      <c r="C61" s="5"/>
+      <c r="C61" s="10"/>
       <c r="D61" s="5"/>
       <c r="G61" s="5"/>
     </row>
@@ -1309,13 +1353,13 @@
     </row>
     <row r="75" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="8"/>
-      <c r="C75" s="10"/>
+      <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="G75" s="5"/>
     </row>
     <row r="76" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="8"/>
-      <c r="C76" s="10"/>
+      <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="G76" s="5"/>
     </row>
@@ -1325,12 +1369,10 @@
       <c r="D77" s="5"/>
       <c r="G77" s="5"/>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="8"/>
       <c r="C78" s="10"/>
       <c r="D78" s="5"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
       <c r="G78" s="5"/>
     </row>
     <row r="79" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1339,10 +1381,12 @@
       <c r="D79" s="5"/>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="8"/>
       <c r="C80" s="10"/>
       <c r="D80" s="5"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
       <c r="G80" s="5"/>
     </row>
     <row r="81" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1357,19 +1401,16 @@
       <c r="D82" s="5"/>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="8"/>
       <c r="C83" s="10"/>
       <c r="D83" s="5"/>
-      <c r="E83" s="7"/>
-      <c r="F83" s="7"/>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G83" s="5"/>
+    </row>
+    <row r="84" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="8"/>
       <c r="C84" s="10"/>
       <c r="D84" s="5"/>
-      <c r="E84" s="7"/>
-      <c r="F84" s="7"/>
       <c r="G84" s="5"/>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
@@ -1378,7 +1419,6 @@
       <c r="D85" s="5"/>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
-      <c r="G85" s="5"/>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="8"/>
@@ -1394,7 +1434,7 @@
       <c r="D87" s="5"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
-      <c r="G87" s="7"/>
+      <c r="G87" s="5"/>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="8"/>
@@ -1402,6 +1442,7 @@
       <c r="D88" s="5"/>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
+      <c r="G88" s="5"/>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="8"/>
@@ -1409,9 +1450,11 @@
       <c r="D89" s="5"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="8"/>
+      <c r="C90" s="10"/>
       <c r="D90" s="5"/>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
@@ -1424,22 +1467,23 @@
       <c r="F91" s="7"/>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="8"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="7"/>
       <c r="F92" s="7"/>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="8"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="7"/>
       <c r="F93" s="7"/>
     </row>
-    <row r="94" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C94" s="5"/>
-      <c r="D94"/>
-      <c r="E94"/>
-      <c r="G94"/>
-    </row>
-    <row r="95" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C95" s="5"/>
-      <c r="D95"/>
-      <c r="E95"/>
-      <c r="G95"/>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F94" s="7"/>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F95" s="7"/>
     </row>
     <row r="96" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C96" s="5"/>
@@ -1463,18 +1507,18 @@
       <c r="C99" s="5"/>
       <c r="D99"/>
       <c r="E99"/>
-      <c r="G99" s="5"/>
+      <c r="G99"/>
     </row>
     <row r="100" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="8"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="5"/>
-      <c r="G100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100"/>
+      <c r="E100"/>
+      <c r="G100"/>
     </row>
     <row r="101" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="8"/>
-      <c r="C101" s="10"/>
-      <c r="D101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101"/>
+      <c r="E101"/>
       <c r="G101" s="5"/>
     </row>
     <row r="102" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1491,13 +1535,13 @@
     </row>
     <row r="104" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="8"/>
-      <c r="C104" s="5"/>
+      <c r="C104" s="10"/>
       <c r="D104" s="5"/>
       <c r="G104" s="5"/>
     </row>
     <row r="105" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B105" s="8"/>
-      <c r="C105" s="5"/>
+      <c r="C105" s="10"/>
       <c r="D105" s="5"/>
       <c r="G105" s="5"/>
     </row>
@@ -1511,42 +1555,40 @@
       <c r="B107" s="8"/>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
       <c r="G107" s="5"/>
     </row>
     <row r="108" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B108" s="8"/>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
-      <c r="E108" s="5"/>
       <c r="G108" s="5"/>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B109" s="8"/>
+      <c r="C109" s="5"/>
       <c r="D109" s="5"/>
       <c r="E109" s="5"/>
-      <c r="F109" s="7"/>
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B110" s="8"/>
+      <c r="C110" s="5"/>
       <c r="D110" s="5"/>
       <c r="E110" s="5"/>
-      <c r="F110" s="7"/>
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" s="8"/>
-      <c r="C111" s="5"/>
       <c r="D111" s="5"/>
       <c r="E111" s="5"/>
+      <c r="F111" s="7"/>
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" s="8"/>
-      <c r="C112" s="5"/>
       <c r="D112" s="5"/>
       <c r="E112" s="5"/>
+      <c r="F112" s="7"/>
       <c r="G112" s="5"/>
     </row>
     <row r="113" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1582,13 +1624,13 @@
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
       <c r="E117" s="5"/>
-      <c r="G117" s="9"/>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G117" s="5"/>
+    </row>
+    <row r="118" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B118" s="8"/>
+      <c r="C118" s="5"/>
       <c r="D118" s="5"/>
       <c r="E118" s="5"/>
-      <c r="F118" s="7"/>
       <c r="G118" s="5"/>
     </row>
     <row r="119" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1596,20 +1638,20 @@
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
       <c r="E119" s="5"/>
-      <c r="G119" s="5"/>
-    </row>
-    <row r="120" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G119" s="9"/>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B120" s="8"/>
-      <c r="C120" s="5"/>
       <c r="D120" s="5"/>
       <c r="E120" s="5"/>
+      <c r="F120" s="7"/>
       <c r="G120" s="5"/>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="8"/>
+      <c r="C121" s="5"/>
       <c r="D121" s="5"/>
       <c r="E121" s="5"/>
-      <c r="F121" s="7"/>
       <c r="G121" s="5"/>
     </row>
     <row r="122" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1626,11 +1668,11 @@
       <c r="F123" s="7"/>
       <c r="G123" s="5"/>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B124" s="8"/>
+      <c r="C124" s="5"/>
       <c r="D124" s="5"/>
       <c r="E124" s="5"/>
-      <c r="F124" s="7"/>
       <c r="G124" s="5"/>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
@@ -1640,47 +1682,47 @@
       <c r="F125" s="7"/>
       <c r="G125" s="5"/>
     </row>
-    <row r="126" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B126" s="8"/>
-      <c r="C126" s="10"/>
       <c r="D126" s="5"/>
       <c r="E126" s="5"/>
+      <c r="F126" s="7"/>
       <c r="G126" s="5"/>
     </row>
-    <row r="127" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B127" s="8"/>
-      <c r="C127" s="10"/>
       <c r="D127" s="5"/>
       <c r="E127" s="5"/>
+      <c r="F127" s="7"/>
       <c r="G127" s="5"/>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B128" s="8"/>
       <c r="C128" s="10"/>
       <c r="D128" s="5"/>
       <c r="E128" s="5"/>
-      <c r="F128" s="7"/>
       <c r="G128" s="5"/>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B129" s="8"/>
+      <c r="C129" s="10"/>
       <c r="D129" s="5"/>
       <c r="E129" s="5"/>
-      <c r="F129" s="7"/>
       <c r="G129" s="5"/>
     </row>
-    <row r="130" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="8"/>
-      <c r="C130" s="5"/>
+      <c r="C130" s="10"/>
       <c r="D130" s="5"/>
       <c r="E130" s="5"/>
+      <c r="F130" s="7"/>
       <c r="G130" s="5"/>
     </row>
-    <row r="131" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B131" s="8"/>
-      <c r="C131" s="5"/>
       <c r="D131" s="5"/>
       <c r="E131" s="5"/>
+      <c r="F131" s="7"/>
       <c r="G131" s="5"/>
     </row>
     <row r="132" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1704,18 +1746,18 @@
       <c r="E134" s="5"/>
       <c r="G134" s="5"/>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B135" s="8"/>
+      <c r="C135" s="5"/>
       <c r="D135" s="5"/>
       <c r="E135" s="5"/>
-      <c r="F135" s="7"/>
       <c r="G135" s="5"/>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B136" s="8"/>
+      <c r="C136" s="5"/>
       <c r="D136" s="5"/>
       <c r="E136" s="5"/>
-      <c r="F136" s="7"/>
       <c r="G136" s="5"/>
     </row>
     <row r="137" spans="2:7" x14ac:dyDescent="0.25">
@@ -1744,12 +1786,14 @@
       <c r="D140" s="5"/>
       <c r="E140" s="5"/>
       <c r="F140" s="7"/>
+      <c r="G140" s="5"/>
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B141" s="8"/>
       <c r="D141" s="5"/>
       <c r="E141" s="5"/>
       <c r="F141" s="7"/>
+      <c r="G141" s="5"/>
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" s="8"/>
@@ -1758,11 +1802,15 @@
       <c r="F142" s="7"/>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B143" s="2"/>
+      <c r="B143" s="8"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="5"/>
       <c r="F143" s="7"/>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B144" s="2"/>
+      <c r="B144" s="8"/>
+      <c r="D144" s="5"/>
+      <c r="E144" s="5"/>
       <c r="F144" s="7"/>
     </row>
     <row r="145" spans="2:7" x14ac:dyDescent="0.25">
@@ -1785,108 +1833,108 @@
       <c r="B149" s="2"/>
       <c r="F149" s="7"/>
     </row>
-    <row r="150" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B150" s="2"/>
-      <c r="C150" s="5"/>
-      <c r="D150"/>
-      <c r="E150"/>
-      <c r="G150"/>
+      <c r="F150" s="7"/>
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B151" s="2"/>
       <c r="F151" s="7"/>
     </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B152" s="2"/>
-      <c r="F152" s="7"/>
-    </row>
-    <row r="153" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C152" s="5"/>
+      <c r="D152"/>
+      <c r="E152"/>
+      <c r="G152"/>
+    </row>
+    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B153" s="2"/>
-      <c r="C153" s="5"/>
-      <c r="D153"/>
-      <c r="E153"/>
-      <c r="G153"/>
-    </row>
-    <row r="154" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F153" s="7"/>
+    </row>
+    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B154" s="2"/>
-      <c r="C154" s="5"/>
-      <c r="D154"/>
-      <c r="E154"/>
-      <c r="G154"/>
-    </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F154" s="7"/>
+    </row>
+    <row r="155" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B155" s="2"/>
-      <c r="F155" s="7"/>
-      <c r="G155" s="7"/>
-    </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C155" s="5"/>
+      <c r="D155"/>
+      <c r="E155"/>
+      <c r="G155"/>
+    </row>
+    <row r="156" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B156" s="2"/>
-      <c r="F156" s="7"/>
+      <c r="C156" s="5"/>
+      <c r="D156"/>
+      <c r="E156"/>
+      <c r="G156"/>
     </row>
     <row r="157" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B157" s="2"/>
       <c r="F157" s="7"/>
+      <c r="G157" s="7"/>
     </row>
     <row r="158" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B158" s="2"/>
-      <c r="D158" s="7"/>
-      <c r="E158" s="7"/>
       <c r="F158" s="7"/>
-      <c r="G158" s="7"/>
     </row>
     <row r="159" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B159" s="2"/>
       <c r="F159" s="7"/>
-      <c r="G159" s="7"/>
     </row>
     <row r="160" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B160" s="2"/>
+      <c r="D160" s="7"/>
+      <c r="E160" s="7"/>
       <c r="F160" s="7"/>
+      <c r="G160" s="7"/>
     </row>
     <row r="161" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B161" s="2"/>
-      <c r="D161" s="7"/>
-      <c r="E161" s="7"/>
       <c r="F161" s="7"/>
+      <c r="G161" s="7"/>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B162" s="2"/>
-      <c r="D162" s="7"/>
-      <c r="E162" s="7"/>
       <c r="F162" s="7"/>
     </row>
     <row r="163" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B163" s="2"/>
-      <c r="D163" s="5"/>
-      <c r="E163" s="5"/>
+      <c r="D163" s="7"/>
+      <c r="E163" s="7"/>
       <c r="F163" s="7"/>
     </row>
     <row r="164" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B164" s="2"/>
+      <c r="D164" s="7"/>
+      <c r="E164" s="7"/>
       <c r="F164" s="7"/>
     </row>
     <row r="165" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B165" s="2"/>
+      <c r="D165" s="5"/>
+      <c r="E165" s="5"/>
       <c r="F165" s="7"/>
     </row>
     <row r="166" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B166" s="2"/>
       <c r="F166" s="7"/>
     </row>
-    <row r="167" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B167" s="2"/>
-      <c r="C167" s="5"/>
-      <c r="D167"/>
-      <c r="E167"/>
-      <c r="G167"/>
+      <c r="F167" s="7"/>
     </row>
     <row r="168" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B168" s="2"/>
       <c r="F168" s="7"/>
     </row>
-    <row r="169" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B169" s="2"/>
-      <c r="F169" s="7"/>
+      <c r="C169" s="5"/>
+      <c r="D169"/>
+      <c r="E169"/>
+      <c r="G169"/>
     </row>
     <row r="170" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B170" s="2"/>
@@ -1899,7 +1947,6 @@
     <row r="172" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B172" s="2"/>
       <c r="F172" s="7"/>
-      <c r="G172" s="7"/>
     </row>
     <row r="173" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B173" s="2"/>
@@ -1908,15 +1955,24 @@
     <row r="174" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B174" s="2"/>
       <c r="F174" s="7"/>
+      <c r="G174" s="7"/>
     </row>
     <row r="175" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B175" s="2"/>
-      <c r="D175" s="5"/>
-      <c r="E175" s="5"/>
       <c r="F175" s="7"/>
     </row>
+    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B176" s="2"/>
+      <c r="F176" s="7"/>
+    </row>
+    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B177" s="2"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="7"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:G172">
+  <autoFilter ref="B1:G174">
     <sortState ref="B2:L87">
       <sortCondition ref="E1:E87"/>
     </sortState>
@@ -1933,7 +1989,7 @@
           <x14:formula1>
             <xm:f>Stats!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>D100:D175 D2:D91</xm:sqref>
+          <xm:sqref>D102:D177 D2:D93</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2037,7 +2093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G15" sqref="G2:H15"/>
     </sheetView>
@@ -2313,15 +2369,15 @@
     </row>
     <row r="9" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
-        <f>Achievements!A9</f>
-        <v>8</v>
+        <f>Achievements!A11</f>
+        <v>10</v>
       </c>
       <c r="B9" s="7" t="str">
-        <f>Achievements!C9</f>
+        <f>Achievements!C11</f>
         <v>Triple Shot</v>
       </c>
       <c r="C9" s="7" t="str">
-        <f>Achievements!F9</f>
+        <f>Achievements!F11</f>
         <v>Maximize the standard shot power</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -2346,15 +2402,15 @@
     </row>
     <row r="10" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <f>Achievements!A10</f>
-        <v>9</v>
+        <f>Achievements!A12</f>
+        <v>11</v>
       </c>
       <c r="B10" s="7" t="str">
-        <f>Achievements!C10</f>
+        <f>Achievements!C12</f>
         <v>Fire Arm</v>
       </c>
       <c r="C10" s="7" t="str">
-        <f>Achievements!F10</f>
+        <f>Achievements!F12</f>
         <v>Upgrade to the firearm shot</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -2379,15 +2435,15 @@
     </row>
     <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
-        <f>Achievements!A11</f>
-        <v>10</v>
+        <f>Achievements!A13</f>
+        <v>12</v>
       </c>
       <c r="B11" s="7" t="str">
-        <f>Achievements!C11</f>
+        <f>Achievements!C13</f>
         <v>Armoured Core</v>
       </c>
       <c r="C11" s="7" t="str">
-        <f>Achievements!F11</f>
+        <f>Achievements!F13</f>
         <v>Have 120 or more health at once</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -2412,15 +2468,15 @@
     </row>
     <row r="12" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <f>Achievements!A12</f>
-        <v>11</v>
+        <f>Achievements!A14</f>
+        <v>13</v>
       </c>
       <c r="B12" s="7" t="str">
-        <f>Achievements!C12</f>
+        <f>Achievements!C14</f>
         <v>Private</v>
       </c>
       <c r="C12" s="7" t="str">
-        <f>Achievements!F12</f>
+        <f>Achievements!F14</f>
         <v>Score more than 100,000 points</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -2445,15 +2501,15 @@
     </row>
     <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
-        <f>Achievements!A13</f>
-        <v>12</v>
+        <f>Achievements!A15</f>
+        <v>14</v>
       </c>
       <c r="B13" s="7" t="str">
-        <f>Achievements!C13</f>
+        <f>Achievements!C15</f>
         <v>Corporal </v>
       </c>
       <c r="C13" s="7" t="str">
-        <f>Achievements!F13</f>
+        <f>Achievements!F15</f>
         <v>Score more than 250,000 points</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -2478,15 +2534,15 @@
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
-        <f>Achievements!A14</f>
-        <v>13</v>
+        <f>Achievements!A16</f>
+        <v>15</v>
       </c>
       <c r="B14" s="7" t="str">
-        <f>Achievements!C14</f>
+        <f>Achievements!C16</f>
         <v>Sergeant </v>
       </c>
       <c r="C14" s="7" t="str">
-        <f>Achievements!F14</f>
+        <f>Achievements!F16</f>
         <v>Score more than 500,000 points</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -2511,15 +2567,15 @@
     </row>
     <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
-        <f>Achievements!A15</f>
-        <v>14</v>
+        <f>Achievements!A17</f>
+        <v>16</v>
       </c>
       <c r="B15" s="7" t="str">
-        <f>Achievements!C15</f>
+        <f>Achievements!C17</f>
         <v>Commander</v>
       </c>
       <c r="C15" s="7" t="str">
-        <f>Achievements!F15</f>
+        <f>Achievements!F17</f>
         <v>Score more than 1,000,000 points</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -2601,8 +2657,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:A76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A10:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2665,55 +2721,55 @@
     <row r="10" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Triple Shot","Maximize the standard shot power", 1, trigger)</v>
+        <v>achievement("Specialized Boss Slayer","Defeat a boss while the special is activated", 5, trigger)</v>
       </c>
     </row>
     <row r="11" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Fire Arm","Upgrade to the firearm shot", 2, trigger)</v>
+        <v>achievement("Nothing Special Here","Defeat a boss without activating the special", 10, trigger)</v>
       </c>
     </row>
     <row r="12" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Armoured Core","Have 120 or more health at once", 3, trigger)</v>
+        <v>achievement("Triple Shot","Maximize the standard shot power", 1, trigger)</v>
       </c>
     </row>
     <row r="13" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Private","Score more than 100,000 points", 5, trigger)</v>
+        <v>achievement("Fire Arm","Upgrade to the firearm shot", 2, trigger)</v>
       </c>
     </row>
     <row r="14" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Corporal ","Score more than 250,000 points", 5, trigger)</v>
+        <v>achievement("Armoured Core","Have 120 or more health at once", 3, trigger)</v>
       </c>
     </row>
     <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Sergeant ","Score more than 500,000 points", 10, trigger)</v>
+        <v>achievement("Private","Score more than 100,000 points", 3, trigger)</v>
       </c>
     </row>
     <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Commander","Score more than 1,000,000 points", 25, trigger)</v>
+        <v>achievement("Corporal ","Score more than 250,000 points", 5, trigger)</v>
       </c>
     </row>
     <row r="17" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("","", , trigger)</v>
+        <v>achievement("Sergeant ","Score more than 500,000 points", 10, trigger)</v>
       </c>
     </row>
     <row r="18" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f ca="1">"achievement("&amp;CHAR(34)&amp;INDIRECT("Achievements!C"&amp;(ROW()-1))&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;INDIRECT("Achievements!F"&amp;(ROW()-1))&amp;CHAR(34)&amp;", "&amp;INDIRECT("Achievements!E"&amp;(ROW()-1))&amp;", trigger)"</f>
-        <v>achievement("","", , trigger)</v>
+        <v>achievement("Commander","Score more than 1,000,000 points", 25, trigger)</v>
       </c>
     </row>
     <row r="19" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3150,7 +3206,7 @@
       </c>
       <c r="G3" s="7">
         <f>SUMIF(Achievements!B:B,E3,Achievements!E:E)</f>
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -3186,18 +3242,18 @@
       </c>
       <c r="C5">
         <f>COUNTIF(Achievements!D:D,A5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>54</v>
       </c>
       <c r="F5" s="4">
         <f>COUNTIF(Achievements!B:B,E5)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G5" s="7">
         <f>SUMIF(Achievements!B:B,E5,Achievements!E:E)</f>
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3239,11 +3295,11 @@
       </c>
       <c r="F7" s="3">
         <f>SUM(F2:F6)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
-        <v>157</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3255,7 +3311,7 @@
       </c>
       <c r="C8">
         <f>COUNTIF(Achievements!D:D,A8)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3289,7 +3345,7 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3">
         <f>SUM(C2:C10)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>